<commit_message>
merge costscale into base, add merra download
</commit_message>
<xml_diff>
--- a/cases-test.xlsx
+++ b/cases-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrown/Dropbox/MITEI/Projects/REGeo/package/REVIEW_Joule/out/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrown/github/zephyr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C491E9A-8C25-7945-8B2A-76AEEF174C5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4A8170-98D3-044B-87A7-FE564D483E7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18320" yWindow="12220" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="144">
   <si>
     <t>case</t>
   </si>
@@ -446,13 +446,19 @@
     <t>life_stor</t>
   </si>
   <si>
-    <t>cfpath</t>
-  </si>
-  <si>
-    <t>v08_states-LCOE-transloss-urbanedge</t>
-  </si>
-  <si>
     <t>ba-base_case303</t>
+  </si>
+  <si>
+    <t>pvscale</t>
+  </si>
+  <si>
+    <t>windscale</t>
+  </si>
+  <si>
+    <t>storscale</t>
+  </si>
+  <si>
+    <t>transscale</t>
   </si>
 </sst>
 </file>
@@ -806,11 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX25"/>
+  <dimension ref="A1:BA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM12" sqref="AM12"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,40 +833,41 @@
     <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.5" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" customWidth="1"/>
-    <col min="15" max="15" width="4.83203125" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" customWidth="1"/>
-    <col min="18" max="19" width="11.33203125" customWidth="1"/>
-    <col min="20" max="21" width="10.5" customWidth="1"/>
-    <col min="22" max="22" width="8" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="8" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" customWidth="1"/>
-    <col min="26" max="26" width="9" customWidth="1"/>
-    <col min="27" max="27" width="9.83203125" customWidth="1"/>
-    <col min="28" max="28" width="12.1640625" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="11.33203125" customWidth="1"/>
-    <col min="32" max="32" width="9.5" customWidth="1"/>
-    <col min="33" max="33" width="10" customWidth="1"/>
-    <col min="34" max="34" width="5.83203125" customWidth="1"/>
-    <col min="35" max="35" width="6.1640625" customWidth="1"/>
-    <col min="36" max="36" width="8.83203125" customWidth="1"/>
-    <col min="37" max="37" width="11" customWidth="1"/>
-    <col min="38" max="38" width="9.33203125" customWidth="1"/>
-    <col min="39" max="39" width="7.5" customWidth="1"/>
-    <col min="40" max="42" width="7.1640625" customWidth="1"/>
-    <col min="43" max="43" width="6.33203125" customWidth="1"/>
-    <col min="44" max="45" width="6.6640625" customWidth="1"/>
-    <col min="46" max="46" width="7.1640625" customWidth="1"/>
-    <col min="47" max="47" width="14.83203125" customWidth="1"/>
-    <col min="48" max="49" width="12.33203125" customWidth="1"/>
-    <col min="50" max="1037" width="10.5" customWidth="1"/>
+    <col min="13" max="16" width="3.5" customWidth="1"/>
+    <col min="17" max="17" width="5.5" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" customWidth="1"/>
+    <col min="19" max="19" width="4.83203125" customWidth="1"/>
+    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.83203125" customWidth="1"/>
+    <col min="22" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="25" width="10.5" customWidth="1"/>
+    <col min="26" max="26" width="8" customWidth="1"/>
+    <col min="27" max="27" width="15" customWidth="1"/>
+    <col min="28" max="28" width="8" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" customWidth="1"/>
+    <col min="30" max="30" width="9" customWidth="1"/>
+    <col min="31" max="31" width="9.83203125" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" customWidth="1"/>
+    <col min="33" max="33" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="11.33203125" customWidth="1"/>
+    <col min="36" max="36" width="9.5" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="38" max="38" width="5.83203125" customWidth="1"/>
+    <col min="39" max="39" width="6.1640625" customWidth="1"/>
+    <col min="40" max="40" width="8.83203125" customWidth="1"/>
+    <col min="41" max="41" width="11" customWidth="1"/>
+    <col min="42" max="42" width="9.33203125" customWidth="1"/>
+    <col min="43" max="43" width="7.5" customWidth="1"/>
+    <col min="44" max="46" width="7.1640625" customWidth="1"/>
+    <col min="47" max="47" width="6.33203125" customWidth="1"/>
+    <col min="48" max="49" width="6.6640625" customWidth="1"/>
+    <col min="50" max="50" width="7.1640625" customWidth="1"/>
+    <col min="51" max="51" width="14.83203125" customWidth="1"/>
+    <col min="52" max="52" width="12.33203125" customWidth="1"/>
+    <col min="53" max="1040" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -898,121 +905,130 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>129</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>130</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>131</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AL1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AM1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AO1" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AP1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AQ1" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AR1" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AS1" t="s">
         <v>137</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AT1" t="s">
         <v>138</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AU1" t="s">
         <v>133</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AV1" t="s">
         <v>134</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AW1" t="s">
         <v>135</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AX1" t="s">
         <v>127</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>36</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AZ1" t="s">
         <v>128</v>
       </c>
-      <c r="AW1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1034,92 +1050,101 @@
       <c r="L2" t="s">
         <v>42</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>43</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>44</v>
       </c>
-      <c r="O2">
+      <c r="S2">
         <v>0.19</v>
       </c>
-      <c r="P2" t="s">
+      <c r="T2" t="s">
         <v>136</v>
       </c>
-      <c r="Q2">
+      <c r="U2">
         <v>100</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
       <c r="V2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
         <v>500</v>
       </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
         <v>0.85</v>
       </c>
-      <c r="AD2">
+      <c r="AH2">
         <v>0.05</v>
       </c>
-      <c r="AE2">
+      <c r="AI2">
         <v>0.05</v>
       </c>
-      <c r="AJ2">
+      <c r="AN2">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK2">
+      <c r="AO2">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AP2" t="s">
         <v>45</v>
       </c>
-      <c r="AQ2">
+      <c r="AU2">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR2">
+      <c r="AV2">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AW2" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT2">
-        <v>1</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="AX2">
+        <v>1</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1141,92 +1166,101 @@
       <c r="L3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>44</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>0.19</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>136</v>
       </c>
-      <c r="Q3">
+      <c r="U3">
         <v>100</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
         <v>500</v>
       </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
         <v>0.85</v>
       </c>
-      <c r="AD3">
+      <c r="AH3">
         <v>0.05</v>
       </c>
-      <c r="AE3">
+      <c r="AI3">
         <v>0.05</v>
       </c>
-      <c r="AJ3">
+      <c r="AN3">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK3">
+      <c r="AO3">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AP3" t="s">
         <v>45</v>
       </c>
-      <c r="AQ3">
+      <c r="AU3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR3">
+      <c r="AV3">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS3" s="2">
+      <c r="AW3" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT3">
-        <v>1</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX3" t="s">
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1248,92 +1282,101 @@
       <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>43</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>44</v>
       </c>
-      <c r="O4">
+      <c r="S4">
         <v>0.19</v>
       </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>136</v>
       </c>
-      <c r="Q4">
+      <c r="U4">
         <v>100</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
       <c r="V4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
         <v>500</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
         <v>0.85</v>
       </c>
-      <c r="AD4">
+      <c r="AH4">
         <v>0.05</v>
       </c>
-      <c r="AE4">
+      <c r="AI4">
         <v>0.05</v>
       </c>
-      <c r="AJ4">
+      <c r="AN4">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK4">
+      <c r="AO4">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AP4" t="s">
         <v>45</v>
       </c>
-      <c r="AQ4">
+      <c r="AU4">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR4">
+      <c r="AV4">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AW4" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT4">
-        <v>1</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX4" t="s">
+      <c r="AX4">
+        <v>1</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1355,92 +1398,101 @@
       <c r="L5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
         <v>43</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>44</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <v>0.19</v>
       </c>
-      <c r="P5" t="s">
+      <c r="T5" t="s">
         <v>136</v>
       </c>
-      <c r="Q5">
+      <c r="U5">
         <v>100</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
       <c r="V5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
         <v>500</v>
       </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
         <v>0.85</v>
       </c>
-      <c r="AD5">
+      <c r="AH5">
         <v>0.05</v>
       </c>
-      <c r="AE5">
+      <c r="AI5">
         <v>0.05</v>
       </c>
-      <c r="AJ5">
+      <c r="AN5">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK5">
+      <c r="AO5">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AP5" t="s">
         <v>45</v>
       </c>
-      <c r="AQ5">
+      <c r="AU5">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR5">
+      <c r="AV5">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AW5" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT5">
-        <v>1</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX5" t="s">
+      <c r="AX5">
+        <v>1</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1462,92 +1514,101 @@
       <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
         <v>43</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
         <v>44</v>
       </c>
-      <c r="O6">
+      <c r="S6">
         <v>0.19</v>
       </c>
-      <c r="P6" t="s">
+      <c r="T6" t="s">
         <v>136</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <v>100</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
       <c r="V6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
         <v>500</v>
       </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
         <v>0.85</v>
       </c>
-      <c r="AD6">
+      <c r="AH6">
         <v>0.05</v>
       </c>
-      <c r="AE6">
+      <c r="AI6">
         <v>0.05</v>
       </c>
-      <c r="AJ6">
+      <c r="AN6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK6">
+      <c r="AO6">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AP6" t="s">
         <v>45</v>
       </c>
-      <c r="AQ6">
+      <c r="AU6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR6">
+      <c r="AV6">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AW6" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT6">
-        <v>1</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX6" t="s">
+      <c r="AX6">
+        <v>1</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1569,92 +1630,101 @@
       <c r="L7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>43</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" t="s">
         <v>44</v>
       </c>
-      <c r="O7">
+      <c r="S7">
         <v>0.19</v>
       </c>
-      <c r="P7" t="s">
+      <c r="T7" t="s">
         <v>136</v>
       </c>
-      <c r="Q7">
+      <c r="U7">
         <v>100</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
       <c r="V7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
         <v>500</v>
       </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
         <v>0.85</v>
       </c>
-      <c r="AD7">
+      <c r="AH7">
         <v>0.05</v>
       </c>
-      <c r="AE7">
+      <c r="AI7">
         <v>0.05</v>
       </c>
-      <c r="AJ7">
+      <c r="AN7">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK7">
+      <c r="AO7">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AP7" t="s">
         <v>45</v>
       </c>
-      <c r="AQ7">
+      <c r="AU7">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR7">
+      <c r="AV7">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AW7" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT7">
-        <v>1</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX7" t="s">
+      <c r="AX7">
+        <v>1</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1676,92 +1746,101 @@
       <c r="L8" t="s">
         <v>42</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
         <v>43</v>
       </c>
-      <c r="N8" t="s">
+      <c r="R8" t="s">
         <v>44</v>
       </c>
-      <c r="O8">
+      <c r="S8">
         <v>0.19</v>
       </c>
-      <c r="P8" t="s">
+      <c r="T8" t="s">
         <v>136</v>
       </c>
-      <c r="Q8">
+      <c r="U8">
         <v>100</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
       <c r="V8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
         <v>500</v>
       </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
         <v>0.85</v>
       </c>
-      <c r="AD8">
+      <c r="AH8">
         <v>0.05</v>
       </c>
-      <c r="AE8">
+      <c r="AI8">
         <v>0.05</v>
       </c>
-      <c r="AJ8">
+      <c r="AN8">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK8">
+      <c r="AO8">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AP8" t="s">
         <v>45</v>
       </c>
-      <c r="AQ8">
+      <c r="AU8">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR8">
+      <c r="AV8">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AW8" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT8">
-        <v>1</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX8" t="s">
+      <c r="AX8">
+        <v>1</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1783,92 +1862,101 @@
       <c r="L9" t="s">
         <v>42</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
         <v>43</v>
       </c>
-      <c r="N9" t="s">
+      <c r="R9" t="s">
         <v>44</v>
       </c>
-      <c r="O9">
+      <c r="S9">
         <v>0.19</v>
       </c>
-      <c r="P9" t="s">
+      <c r="T9" t="s">
         <v>136</v>
       </c>
-      <c r="Q9">
+      <c r="U9">
         <v>100</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
       <c r="V9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
         <v>500</v>
       </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
       <c r="AB9">
         <v>0</v>
       </c>
       <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
         <v>0.85</v>
       </c>
-      <c r="AD9">
+      <c r="AH9">
         <v>0.05</v>
       </c>
-      <c r="AE9">
+      <c r="AI9">
         <v>0.05</v>
       </c>
-      <c r="AJ9">
+      <c r="AN9">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK9">
+      <c r="AO9">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AP9" t="s">
         <v>45</v>
       </c>
-      <c r="AQ9">
+      <c r="AU9">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR9">
+      <c r="AV9">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AW9" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT9">
-        <v>1</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX9" t="s">
+      <c r="AX9">
+        <v>1</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1890,92 +1978,101 @@
       <c r="L10" t="s">
         <v>42</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
         <v>43</v>
       </c>
-      <c r="N10" t="s">
+      <c r="R10" t="s">
         <v>44</v>
       </c>
-      <c r="O10">
+      <c r="S10">
         <v>0.19</v>
       </c>
-      <c r="P10" t="s">
+      <c r="T10" t="s">
         <v>136</v>
       </c>
-      <c r="Q10">
+      <c r="U10">
         <v>100</v>
       </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
       <c r="V10">
         <v>1</v>
       </c>
       <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
         <v>500</v>
       </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
       <c r="AB10">
         <v>0</v>
       </c>
       <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
         <v>0.85</v>
       </c>
-      <c r="AD10">
+      <c r="AH10">
         <v>0.05</v>
       </c>
-      <c r="AE10">
+      <c r="AI10">
         <v>0.05</v>
       </c>
-      <c r="AJ10">
+      <c r="AN10">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK10">
+      <c r="AO10">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AP10" t="s">
         <v>45</v>
       </c>
-      <c r="AQ10">
+      <c r="AU10">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR10">
+      <c r="AV10">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS10" s="2">
+      <c r="AW10" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT10">
-        <v>1</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX10" t="s">
+      <c r="AX10">
+        <v>1</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1997,92 +2094,101 @@
       <c r="L11" t="s">
         <v>42</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
         <v>43</v>
       </c>
-      <c r="N11" t="s">
+      <c r="R11" t="s">
         <v>44</v>
       </c>
-      <c r="O11">
+      <c r="S11">
         <v>0.19</v>
       </c>
-      <c r="P11" t="s">
+      <c r="T11" t="s">
         <v>136</v>
       </c>
-      <c r="Q11">
+      <c r="U11">
         <v>100</v>
       </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
       <c r="V11">
         <v>1</v>
       </c>
       <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
         <v>500</v>
       </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
       <c r="AB11">
         <v>0</v>
       </c>
       <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
         <v>0.85</v>
       </c>
-      <c r="AD11">
+      <c r="AH11">
         <v>0.05</v>
       </c>
-      <c r="AE11">
+      <c r="AI11">
         <v>0.05</v>
       </c>
-      <c r="AJ11">
+      <c r="AN11">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK11">
+      <c r="AO11">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AP11" t="s">
         <v>45</v>
       </c>
-      <c r="AQ11">
+      <c r="AU11">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR11">
+      <c r="AV11">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AW11" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT11">
-        <v>1</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX11" t="s">
+      <c r="AX11">
+        <v>1</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2104,92 +2210,101 @@
       <c r="L12" t="s">
         <v>42</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
         <v>43</v>
       </c>
-      <c r="N12" t="s">
+      <c r="R12" t="s">
         <v>44</v>
       </c>
-      <c r="O12">
+      <c r="S12">
         <v>0.19</v>
       </c>
-      <c r="P12" t="s">
+      <c r="T12" t="s">
         <v>136</v>
       </c>
-      <c r="Q12">
+      <c r="U12">
         <v>100</v>
       </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="S12">
-        <v>1</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
       <c r="V12">
         <v>1</v>
       </c>
       <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
         <v>500</v>
       </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
       <c r="AB12">
         <v>0</v>
       </c>
       <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
         <v>0.85</v>
       </c>
-      <c r="AD12">
+      <c r="AH12">
         <v>0.05</v>
       </c>
-      <c r="AE12">
+      <c r="AI12">
         <v>0.05</v>
       </c>
-      <c r="AJ12">
+      <c r="AN12">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK12">
+      <c r="AO12">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AP12" t="s">
         <v>45</v>
       </c>
-      <c r="AQ12">
+      <c r="AU12">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR12">
+      <c r="AV12">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AW12" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT12">
-        <v>1</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX12" t="s">
+      <c r="AX12">
+        <v>1</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2211,92 +2326,101 @@
       <c r="L13" t="s">
         <v>42</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
         <v>43</v>
       </c>
-      <c r="N13" t="s">
+      <c r="R13" t="s">
         <v>44</v>
       </c>
-      <c r="O13">
+      <c r="S13">
         <v>0.19</v>
       </c>
-      <c r="P13" t="s">
+      <c r="T13" t="s">
         <v>136</v>
       </c>
-      <c r="Q13">
+      <c r="U13">
         <v>100</v>
       </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
-        <v>1</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
       <c r="V13">
         <v>1</v>
       </c>
       <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
         <v>500</v>
       </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
       <c r="AB13">
         <v>0</v>
       </c>
       <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
         <v>0.85</v>
       </c>
-      <c r="AD13">
+      <c r="AH13">
         <v>0.05</v>
       </c>
-      <c r="AE13">
+      <c r="AI13">
         <v>0.05</v>
       </c>
-      <c r="AJ13">
+      <c r="AN13">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK13">
+      <c r="AO13">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="AP13" t="s">
         <v>45</v>
       </c>
-      <c r="AQ13">
+      <c r="AU13">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR13">
+      <c r="AV13">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AW13" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT13">
-        <v>1</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX13" t="s">
+      <c r="AX13">
+        <v>1</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2318,92 +2442,101 @@
       <c r="L14" t="s">
         <v>42</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
         <v>43</v>
       </c>
-      <c r="N14" t="s">
+      <c r="R14" t="s">
         <v>44</v>
       </c>
-      <c r="O14">
+      <c r="S14">
         <v>0.19</v>
       </c>
-      <c r="P14" t="s">
+      <c r="T14" t="s">
         <v>136</v>
       </c>
-      <c r="Q14">
+      <c r="U14">
         <v>100</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>1</v>
-      </c>
       <c r="V14">
         <v>1</v>
       </c>
       <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
         <v>500</v>
       </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
       <c r="AB14">
         <v>0</v>
       </c>
       <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
         <v>0.85</v>
       </c>
-      <c r="AD14">
+      <c r="AH14">
         <v>0.05</v>
       </c>
-      <c r="AE14">
+      <c r="AI14">
         <v>0.05</v>
       </c>
-      <c r="AJ14">
+      <c r="AN14">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK14">
+      <c r="AO14">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AP14" t="s">
         <v>45</v>
       </c>
-      <c r="AQ14">
+      <c r="AU14">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR14">
+      <c r="AV14">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS14" s="2">
+      <c r="AW14" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT14">
-        <v>1</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX14" t="s">
+      <c r="AX14">
+        <v>1</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2425,92 +2558,101 @@
       <c r="L15" t="s">
         <v>42</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
         <v>43</v>
       </c>
-      <c r="N15" t="s">
+      <c r="R15" t="s">
         <v>44</v>
       </c>
-      <c r="O15">
+      <c r="S15">
         <v>0.19</v>
       </c>
-      <c r="P15" t="s">
+      <c r="T15" t="s">
         <v>136</v>
       </c>
-      <c r="Q15">
+      <c r="U15">
         <v>100</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
       <c r="V15">
         <v>1</v>
       </c>
       <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
         <v>500</v>
       </c>
-      <c r="X15">
-        <v>0</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
       <c r="AB15">
         <v>0</v>
       </c>
       <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
         <v>0.85</v>
       </c>
-      <c r="AD15">
+      <c r="AH15">
         <v>0.05</v>
       </c>
-      <c r="AE15">
+      <c r="AI15">
         <v>0.05</v>
       </c>
-      <c r="AJ15">
+      <c r="AN15">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK15">
+      <c r="AO15">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AP15" t="s">
         <v>45</v>
       </c>
-      <c r="AQ15">
+      <c r="AU15">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR15">
+      <c r="AV15">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS15" s="2">
+      <c r="AW15" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT15">
-        <v>1</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX15" t="s">
+      <c r="AX15">
+        <v>1</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2532,92 +2674,101 @@
       <c r="L16" t="s">
         <v>42</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
         <v>43</v>
       </c>
-      <c r="N16" t="s">
+      <c r="R16" t="s">
         <v>44</v>
       </c>
-      <c r="O16">
+      <c r="S16">
         <v>0.19</v>
       </c>
-      <c r="P16" t="s">
+      <c r="T16" t="s">
         <v>136</v>
       </c>
-      <c r="Q16">
+      <c r="U16">
         <v>100</v>
       </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
       <c r="V16">
         <v>1</v>
       </c>
       <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
         <v>500</v>
       </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <v>0</v>
-      </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
         <v>0.85</v>
       </c>
-      <c r="AD16">
+      <c r="AH16">
         <v>0.05</v>
       </c>
-      <c r="AE16">
+      <c r="AI16">
         <v>0.05</v>
       </c>
-      <c r="AJ16">
+      <c r="AN16">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK16">
+      <c r="AO16">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AP16" t="s">
         <v>45</v>
       </c>
-      <c r="AQ16">
+      <c r="AU16">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR16">
+      <c r="AV16">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AW16" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT16">
-        <v>1</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW16" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX16" t="s">
+      <c r="AX16">
+        <v>1</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2639,92 +2790,101 @@
       <c r="L17" t="s">
         <v>42</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
         <v>43</v>
       </c>
-      <c r="N17" t="s">
+      <c r="R17" t="s">
         <v>44</v>
       </c>
-      <c r="O17">
+      <c r="S17">
         <v>0.19</v>
       </c>
-      <c r="P17" t="s">
+      <c r="T17" t="s">
         <v>136</v>
       </c>
-      <c r="Q17">
+      <c r="U17">
         <v>100</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
-      </c>
       <c r="V17">
         <v>1</v>
       </c>
       <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
         <v>500</v>
       </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
         <v>0.85</v>
       </c>
-      <c r="AD17">
+      <c r="AH17">
         <v>0.05</v>
       </c>
-      <c r="AE17">
+      <c r="AI17">
         <v>0.05</v>
       </c>
-      <c r="AJ17">
+      <c r="AN17">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK17">
+      <c r="AO17">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL17" t="s">
+      <c r="AP17" t="s">
         <v>45</v>
       </c>
-      <c r="AQ17">
+      <c r="AU17">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR17">
+      <c r="AV17">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS17" s="2">
+      <c r="AW17" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT17">
-        <v>1</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX17" t="s">
+      <c r="AX17">
+        <v>1</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2746,92 +2906,101 @@
       <c r="L18" t="s">
         <v>42</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
         <v>43</v>
       </c>
-      <c r="N18" t="s">
+      <c r="R18" t="s">
         <v>44</v>
       </c>
-      <c r="O18">
+      <c r="S18">
         <v>0.19</v>
       </c>
-      <c r="P18" t="s">
+      <c r="T18" t="s">
         <v>136</v>
       </c>
-      <c r="Q18">
+      <c r="U18">
         <v>100</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
       <c r="V18">
         <v>1</v>
       </c>
       <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
         <v>500</v>
       </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
       <c r="AB18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
         <v>0.85</v>
       </c>
-      <c r="AD18">
+      <c r="AH18">
         <v>0.05</v>
       </c>
-      <c r="AE18">
+      <c r="AI18">
         <v>0.05</v>
       </c>
-      <c r="AJ18">
+      <c r="AN18">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK18">
+      <c r="AO18">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AP18" t="s">
         <v>45</v>
       </c>
-      <c r="AQ18">
+      <c r="AU18">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR18">
+      <c r="AV18">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS18" s="2">
+      <c r="AW18" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT18">
-        <v>1</v>
-      </c>
-      <c r="AU18" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW18" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX18" t="s">
+      <c r="AX18">
+        <v>1</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2853,92 +3022,101 @@
       <c r="L19" t="s">
         <v>42</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
         <v>43</v>
       </c>
-      <c r="N19" t="s">
+      <c r="R19" t="s">
         <v>44</v>
       </c>
-      <c r="O19">
+      <c r="S19">
         <v>0.19</v>
       </c>
-      <c r="P19" t="s">
+      <c r="T19" t="s">
         <v>136</v>
       </c>
-      <c r="Q19">
+      <c r="U19">
         <v>100</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
       <c r="V19">
         <v>1</v>
       </c>
       <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
         <v>500</v>
       </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <v>0</v>
-      </c>
       <c r="AB19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
         <v>0.85</v>
       </c>
-      <c r="AD19">
+      <c r="AH19">
         <v>0.05</v>
       </c>
-      <c r="AE19">
+      <c r="AI19">
         <v>0.05</v>
       </c>
-      <c r="AJ19">
+      <c r="AN19">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK19">
+      <c r="AO19">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AP19" t="s">
         <v>45</v>
       </c>
-      <c r="AQ19">
+      <c r="AU19">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR19">
+      <c r="AV19">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS19" s="2">
+      <c r="AW19" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT19">
-        <v>1</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW19" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX19" t="s">
+      <c r="AX19">
+        <v>1</v>
+      </c>
+      <c r="AY19" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2960,92 +3138,101 @@
       <c r="L20" t="s">
         <v>42</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
         <v>43</v>
       </c>
-      <c r="N20" t="s">
+      <c r="R20" t="s">
         <v>44</v>
       </c>
-      <c r="O20">
+      <c r="S20">
         <v>0.19</v>
       </c>
-      <c r="P20" t="s">
+      <c r="T20" t="s">
         <v>136</v>
       </c>
-      <c r="Q20">
+      <c r="U20">
         <v>100</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>1</v>
-      </c>
       <c r="V20">
         <v>1</v>
       </c>
       <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
         <v>500</v>
       </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="AA20">
-        <v>0</v>
-      </c>
       <c r="AB20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
         <v>0.85</v>
       </c>
-      <c r="AD20">
+      <c r="AH20">
         <v>0.05</v>
       </c>
-      <c r="AE20">
+      <c r="AI20">
         <v>0.05</v>
       </c>
-      <c r="AJ20">
+      <c r="AN20">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK20">
+      <c r="AO20">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL20" t="s">
+      <c r="AP20" t="s">
         <v>45</v>
       </c>
-      <c r="AQ20">
+      <c r="AU20">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR20">
+      <c r="AV20">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS20" s="2">
+      <c r="AW20" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT20">
-        <v>1</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX20" t="s">
+      <c r="AX20">
+        <v>1</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3067,92 +3254,101 @@
       <c r="L21" t="s">
         <v>42</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
         <v>43</v>
       </c>
-      <c r="N21" t="s">
+      <c r="R21" t="s">
         <v>44</v>
       </c>
-      <c r="O21">
+      <c r="S21">
         <v>0.19</v>
       </c>
-      <c r="P21" t="s">
+      <c r="T21" t="s">
         <v>136</v>
       </c>
-      <c r="Q21">
+      <c r="U21">
         <v>100</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
       <c r="V21">
         <v>1</v>
       </c>
       <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
         <v>500</v>
       </c>
-      <c r="X21">
-        <v>1</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
       <c r="AB21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
         <v>0.85</v>
       </c>
-      <c r="AD21">
+      <c r="AH21">
         <v>0.05</v>
       </c>
-      <c r="AE21">
+      <c r="AI21">
         <v>0.05</v>
       </c>
-      <c r="AJ21">
+      <c r="AN21">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK21">
+      <c r="AO21">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AP21" t="s">
         <v>45</v>
       </c>
-      <c r="AQ21">
+      <c r="AU21">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR21">
+      <c r="AV21">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS21" s="2">
+      <c r="AW21" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT21">
-        <v>1</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX21" t="s">
+      <c r="AX21">
+        <v>1</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3174,92 +3370,101 @@
       <c r="L22" t="s">
         <v>42</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
         <v>43</v>
       </c>
-      <c r="N22" t="s">
+      <c r="R22" t="s">
         <v>44</v>
       </c>
-      <c r="O22">
+      <c r="S22">
         <v>0.19</v>
       </c>
-      <c r="P22" t="s">
+      <c r="T22" t="s">
         <v>136</v>
       </c>
-      <c r="Q22">
+      <c r="U22">
         <v>100</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
       <c r="V22">
         <v>1</v>
       </c>
       <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
         <v>500</v>
       </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <v>0</v>
-      </c>
       <c r="AB22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
         <v>0.85</v>
       </c>
-      <c r="AD22">
+      <c r="AH22">
         <v>0.05</v>
       </c>
-      <c r="AE22">
+      <c r="AI22">
         <v>0.05</v>
       </c>
-      <c r="AJ22">
+      <c r="AN22">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK22">
+      <c r="AO22">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AP22" t="s">
         <v>45</v>
       </c>
-      <c r="AQ22">
+      <c r="AU22">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR22">
+      <c r="AV22">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS22" s="2">
+      <c r="AW22" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT22">
-        <v>1</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX22" t="s">
+      <c r="AX22">
+        <v>1</v>
+      </c>
+      <c r="AY22" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3281,92 +3486,101 @@
       <c r="L23" t="s">
         <v>42</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
         <v>43</v>
       </c>
-      <c r="N23" t="s">
+      <c r="R23" t="s">
         <v>44</v>
       </c>
-      <c r="O23">
+      <c r="S23">
         <v>0.19</v>
       </c>
-      <c r="P23" t="s">
+      <c r="T23" t="s">
         <v>136</v>
       </c>
-      <c r="Q23">
+      <c r="U23">
         <v>100</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
       <c r="V23">
         <v>1</v>
       </c>
       <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
         <v>500</v>
       </c>
-      <c r="X23">
-        <v>1</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
-      <c r="AA23">
-        <v>0</v>
-      </c>
       <c r="AB23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
         <v>0.85</v>
       </c>
-      <c r="AD23">
+      <c r="AH23">
         <v>0.05</v>
       </c>
-      <c r="AE23">
+      <c r="AI23">
         <v>0.05</v>
       </c>
-      <c r="AJ23">
+      <c r="AN23">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK23">
+      <c r="AO23">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL23" t="s">
+      <c r="AP23" t="s">
         <v>45</v>
       </c>
-      <c r="AQ23">
+      <c r="AU23">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR23">
+      <c r="AV23">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS23" s="2">
+      <c r="AW23" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT23">
-        <v>1</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX23" t="s">
+      <c r="AX23">
+        <v>1</v>
+      </c>
+      <c r="AY23" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3388,92 +3602,101 @@
       <c r="L24" t="s">
         <v>42</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
         <v>43</v>
       </c>
-      <c r="N24" t="s">
+      <c r="R24" t="s">
         <v>44</v>
       </c>
-      <c r="O24">
+      <c r="S24">
         <v>0.19</v>
       </c>
-      <c r="P24" t="s">
+      <c r="T24" t="s">
         <v>136</v>
       </c>
-      <c r="Q24">
+      <c r="U24">
         <v>100</v>
       </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
       <c r="V24">
         <v>1</v>
       </c>
       <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
         <v>500</v>
       </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
-      </c>
-      <c r="AA24">
-        <v>0</v>
-      </c>
       <c r="AB24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
         <v>0.85</v>
       </c>
-      <c r="AD24">
+      <c r="AH24">
         <v>0.05</v>
       </c>
-      <c r="AE24">
+      <c r="AI24">
         <v>0.05</v>
       </c>
-      <c r="AJ24">
+      <c r="AN24">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK24">
+      <c r="AO24">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL24" t="s">
+      <c r="AP24" t="s">
         <v>45</v>
       </c>
-      <c r="AQ24">
+      <c r="AU24">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR24">
+      <c r="AV24">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS24" s="2">
+      <c r="AW24" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT24">
-        <v>1</v>
-      </c>
-      <c r="AU24" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW24" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX24" t="s">
+      <c r="AX24">
+        <v>1</v>
+      </c>
+      <c r="AY24" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3495,88 +3718,97 @@
       <c r="L25" t="s">
         <v>42</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
         <v>43</v>
       </c>
-      <c r="N25" t="s">
+      <c r="R25" t="s">
         <v>44</v>
       </c>
-      <c r="O25">
+      <c r="S25">
         <v>0.19</v>
       </c>
-      <c r="P25" t="s">
+      <c r="T25" t="s">
         <v>136</v>
       </c>
-      <c r="Q25">
+      <c r="U25">
         <v>100</v>
       </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
       <c r="V25">
         <v>1</v>
       </c>
       <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
         <v>500</v>
       </c>
-      <c r="X25">
-        <v>1</v>
-      </c>
-      <c r="Y25">
-        <v>0</v>
-      </c>
-      <c r="AA25">
-        <v>0</v>
-      </c>
       <c r="AB25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
         <v>0.85</v>
       </c>
-      <c r="AD25">
+      <c r="AH25">
         <v>0.05</v>
       </c>
-      <c r="AE25">
+      <c r="AI25">
         <v>0.05</v>
       </c>
-      <c r="AJ25">
+      <c r="AN25">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AK25">
+      <c r="AO25">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="AL25" t="s">
+      <c r="AP25" t="s">
         <v>45</v>
       </c>
-      <c r="AQ25">
+      <c r="AU25">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="AR25">
+      <c r="AV25">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="AS25" s="2">
+      <c r="AW25" s="2">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="AT25">
-        <v>1</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>141</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>140</v>
-      </c>
-      <c r="AX25" t="s">
+      <c r="AX25">
+        <v>1</v>
+      </c>
+      <c r="AY25" t="s">
+        <v>139</v>
+      </c>
+      <c r="BA25" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>